<commit_message>
FINFLUX-2698 Correcting Overdue failed scenarios
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/5038-Nabkisan-Componding-penality-Charge-loan-2ndInstallment.xlsx
+++ b/Finflux Automation Excels/Client/5038-Nabkisan-Componding-penality-Charge-loan-2ndInstallment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Modify Transaction1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="79">
   <si>
     <t>OverDueTillDate</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Over Due</t>
   </si>
   <si>
-    <t>Principal</t>
-  </si>
-  <si>
     <t>Interest</t>
   </si>
   <si>
@@ -262,13 +259,22 @@
   </si>
   <si>
     <t>$ 44.38</t>
+  </si>
+  <si>
+    <t>$ 51.92</t>
+  </si>
+  <si>
+    <t>$ 0.07</t>
+  </si>
+  <si>
+    <t>$ 0.08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +301,36 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -329,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -351,7 +387,27 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -689,138 +745,138 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="8">
         <v>42004</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="8">
         <v>42004</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="8">
         <v>42004</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="8">
         <v>42004</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="G5" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" s="6"/>
     </row>
@@ -841,85 +897,85 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="8">
         <v>42035</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="8">
         <v>42035</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -942,85 +998,85 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="8">
         <v>42063</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="8">
         <v>42063</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1043,85 +1099,85 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="8">
         <v>42094</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="8">
         <v>42094</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1134,7 +1190,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1235,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>300.95999999999998</v>
+        <v>301.18</v>
       </c>
       <c r="B3" s="6">
         <v>0</v>
@@ -1191,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>300.95999999999998</v>
+        <v>301.18</v>
       </c>
       <c r="F3" s="6">
         <v>165.6</v>
@@ -1247,7 +1303,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,22 +1313,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
@@ -1441,7 +1497,7 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,45 +1507,45 @@
   <sheetData>
     <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="4"/>
       <c r="N1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="P1" s="4"/>
       <c r="Q1" s="4" t="s">
@@ -1628,13 +1684,13 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6">
-        <v>835.73</v>
+        <v>835.72</v>
       </c>
       <c r="G5" s="7">
-        <v>2489.66</v>
+        <v>2489.67</v>
       </c>
       <c r="H5" s="6">
-        <v>51.99</v>
+        <v>52</v>
       </c>
       <c r="I5" s="6">
         <v>0</v>
@@ -1673,13 +1729,13 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6">
-        <v>835.2</v>
+        <v>835.13</v>
       </c>
       <c r="G6" s="7">
-        <v>1654.46</v>
+        <v>1654.54</v>
       </c>
       <c r="H6" s="6">
-        <v>52.52</v>
+        <v>52.59</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
@@ -1718,13 +1774,13 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6">
-        <v>839.8</v>
+        <v>839.73</v>
       </c>
       <c r="G7" s="6">
-        <v>814.66</v>
+        <v>814.81</v>
       </c>
       <c r="H7" s="6">
-        <v>47.92</v>
+        <v>47.99</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
@@ -1763,13 +1819,13 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6">
-        <v>814.66</v>
+        <v>814.81</v>
       </c>
       <c r="G8" s="6">
         <v>0</v>
       </c>
       <c r="H8" s="6">
-        <v>47.7</v>
+        <v>47.77</v>
       </c>
       <c r="I8" s="6">
         <v>0</v>
@@ -1778,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="6">
-        <v>862.36</v>
+        <v>862.58</v>
       </c>
       <c r="L8" s="6">
         <v>0</v>
@@ -1792,7 +1848,7 @@
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="6">
-        <v>862.36</v>
+        <v>862.58</v>
       </c>
     </row>
   </sheetData>
@@ -1802,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,75 +1871,67 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>158</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="8">
         <v>42094</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="6">
-        <v>53.47</v>
+        <v>53.55</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="7">
-        <v>5299.83</v>
+        <v>5307.35</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>157</v>
+        <v>62</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="8">
         <v>42094</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="6">
-        <v>53.47</v>
+        <v>0.08</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1895,91 +1943,91 @@
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>156</v>
+        <v>54</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="8">
+        <v>42094</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="8">
-        <v>42063</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E4" s="6">
-        <v>47.86</v>
+        <v>53.47</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="7">
-        <v>5246.36</v>
+      <c r="J4" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>155</v>
+        <v>61</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="8">
         <v>42063</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E5" s="6">
-        <v>47.86</v>
+        <v>47.93</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="6">
-        <v>0</v>
+      <c r="J5" s="7">
+        <v>5253.8</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>154</v>
+        <v>60</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="8">
+        <v>42063</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="8">
-        <v>42035</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E6" s="6">
-        <v>52.45</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="7">
-        <v>5198.5</v>
+      <c r="J6" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>153</v>
+        <v>52</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="8">
+        <v>42063</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="8">
-        <v>42035</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="E7" s="6">
-        <v>52.45</v>
+        <v>47.86</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1991,139 +2039,139 @@
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>160</v>
+        <v>59</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="8">
-        <v>42004</v>
+        <v>42035</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E8" s="6">
-        <v>51.92</v>
+        <v>52.52</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="6">
-        <v>0</v>
+      <c r="J8" s="7">
+        <v>5205.87</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>152</v>
+        <v>58</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="8">
+        <v>42035</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="8">
-        <v>42004</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E9" s="6">
-        <v>51.92</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="7">
-        <v>5146.05</v>
+      <c r="J9" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="8">
+        <v>42035</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="8">
-        <v>41973</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E10" s="6">
-        <v>49.75</v>
+        <v>52.45</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="7">
-        <v>5094.13</v>
+      <c r="J10" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="8">
-        <v>41973</v>
+        <v>42004</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E11" s="6">
-        <v>49.75</v>
+        <v>59.22</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="6">
-        <v>0</v>
+      <c r="J11" s="7">
+        <v>5153.3500000000004</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="8">
+        <v>42004</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="8">
-        <v>41943</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E12" s="6">
-        <v>44.38</v>
+        <v>7.3</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="7">
-        <v>5044.38</v>
+      <c r="J12" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
-        <v>147</v>
+        <v>48</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="8">
+        <v>42004</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="8">
-        <v>41943</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="E13" s="6">
-        <v>44.38</v>
+        <v>51.92</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -2135,25 +2183,121 @@
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
-        <v>146</v>
+        <v>47</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="8">
+        <v>41973</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="6">
+        <v>49.75</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="7">
+        <v>5094.13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>46</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="8">
+        <v>41973</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="8">
+      <c r="E15" s="6">
+        <v>49.75</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>45</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="8">
+        <v>41943</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="6">
+        <v>44.38</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7">
+        <v>5044.38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>44</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="8">
+        <v>41943</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="6">
+        <v>44.38</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>43</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="8">
         <v>41917</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="D18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="5">
         <v>5000</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5">
         <v>5000</v>
       </c>
     </row>
@@ -2177,23 +2321,23 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>6</v>
@@ -2205,7 +2349,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2223,32 +2367,32 @@
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="8">
         <v>41978</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="I3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2268,85 +2412,85 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="8">
         <v>41917</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="H2" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="8">
         <v>41917</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2356,367 +2500,579 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="14"/>
+    <col min="3" max="3" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="14"/>
+    <col min="7" max="7" width="12.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="16">
+        <v>41943</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="8">
+      <c r="H2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="16">
         <v>41943</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="16">
+        <v>41973</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="H5" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="16">
+        <v>41973</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="G6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="15"/>
+      <c r="I6" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="16">
+        <v>42004</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="16">
+        <v>42004</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="F9" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="16">
+        <v>42004</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="16">
+        <v>42004</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="16">
+        <v>42035</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="8">
-        <v>41943</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="H14" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="16">
+        <v>42035</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="15"/>
+      <c r="I15" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="16">
+        <v>42035</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="H17" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="16">
+        <v>42035</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="I18" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="16">
+        <v>42063</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="16">
+        <v>42063</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" s="15"/>
+      <c r="I21" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="8">
-        <v>41973</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="B23" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="16">
+        <v>42063</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E23" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="16">
+        <v>42063</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="16">
+        <v>42094</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="G26" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="16">
+        <v>42094</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="F27" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="15"/>
+      <c r="I27" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="8">
-        <v>41973</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="B29" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="16">
+        <v>42094</v>
+      </c>
+      <c r="D29" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E29" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="16">
+        <v>42094</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="8">
-        <v>42004</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="8">
-        <v>42004</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="8">
-        <v>42035</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="8">
-        <v>42035</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="8">
-        <v>42063</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="8">
-        <v>42063</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="8">
-        <v>42094</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="8">
-        <v>42094</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="9" t="s">
-        <v>75</v>
+      <c r="I30" s="17" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2729,96 +3085,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="10"/>
+    <col min="3" max="3" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="8">
+      <c r="A2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="12">
         <v>41973</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12">
+        <v>41973</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="8">
-        <v>41973</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>70</v>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>